<commit_message>
Se actualizó la información en méticas y retrospectiva
</commit_message>
<xml_diff>
--- a/Métricas.xlsx
+++ b/Métricas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Magaly Peña\Documents\Juego-Donde\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Magaly Peña\Desktop\donde-web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F6B945-DC41-447B-8C0A-1B906B4C95E4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94A0B2B-84A2-414A-8524-08EEB8ABEDBC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1560FA2C-DEF1-40A9-9EDB-C007F191B209}"/>
   </bookViews>
@@ -2758,7 +2758,7 @@
   <dimension ref="A1:AU217"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3727,11 +3727,11 @@
         <v>88</v>
       </c>
       <c r="P12" s="28">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="Q12" s="32">
         <f t="shared" si="0"/>
-        <v>1.4545454545454546</v>
+        <v>1.6590909090909092</v>
       </c>
       <c r="R12" s="28"/>
       <c r="S12" s="28"/>
@@ -3792,11 +3792,11 @@
         <v>48</v>
       </c>
       <c r="AT12" s="28">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="AU12" s="33">
         <f>AT12/AS12</f>
-        <v>1.75</v>
+        <v>2.125</v>
       </c>
     </row>
     <row r="13" spans="1:47" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>